<commit_message>
Update Molpay SGD Fee Exception & Upload Bucket Stg Config
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_Expedia/Data/ListReport.xlsx
+++ b/Traveloka_DataAutomation_Portal_Expedia/Data/ListReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\Traveloka_DataAutomation_Portal_Expedia\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Portal_Expedia\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E050FB4D-F012-421D-B22F-E411E516369D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128D40D2-F5FF-4010-A4AF-BFE471C4B9C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2316" yWindow="2316" windowWidth="16308" windowHeight="7776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23232" windowHeight="11496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -408,16 +408,16 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G4"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" style="1" bestFit="1"/>
+    <col min="4" max="4" width="19.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.25" bestFit="1" customWidth="1"/>
   </cols>
@@ -487,7 +487,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Update expedia after UAT | Not finalized
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_Expedia/Data/ListReport.xlsx
+++ b/Traveloka_DataAutomation_Portal_Expedia/Data/ListReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Portal_Expedia\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128D40D2-F5FF-4010-A4AF-BFE471C4B9C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0771C9B5-D7AE-4775-94F1-F792607A0639}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23232" windowHeight="11496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="984" yWindow="12852" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>BPID</t>
   </si>
@@ -77,6 +77,15 @@
   </si>
   <si>
     <t>Business Model Name</t>
+  </si>
+  <si>
+    <t>Expedia Credit Limit_Marketing Fee</t>
+  </si>
+  <si>
+    <t>Marketing Fee Amsterdam (Pay Hotel Expedia)</t>
+  </si>
+  <si>
+    <t>Expedia Marketing Fee Penalty</t>
   </si>
 </sst>
 </file>
@@ -405,24 +414,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49" style="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,86 +440,69 @@
         <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>609406</v>
       </c>
-      <c r="D2"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>505992</v>
       </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C4">
-        <v>505992</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1" t="s">
+        <v>461953</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <customProperties>
+    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -524,10 +514,10 @@
       <selection sqref="A1:G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.625" style="1" customWidth="1"/>
-    <col min="3" max="5" width="11.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" style="1" customWidth="1"/>
+    <col min="3" max="5" width="11.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -621,5 +611,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <customProperties>
+    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId1"/>
+  </customProperties>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update expedia report 4*, 5*, 6*
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_Expedia/Data/ListReport.xlsx
+++ b/Traveloka_DataAutomation_Portal_Expedia/Data/ListReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Portal_Expedia\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0771C9B5-D7AE-4775-94F1-F792607A0639}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF96517-4FDB-4DAC-84FA-56EA3D55ACBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="984" yWindow="12852" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3852" yWindow="3852" windowWidth="21588" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -79,13 +79,13 @@
     <t>Business Model Name</t>
   </si>
   <si>
-    <t>Expedia Credit Limit_Marketing Fee</t>
-  </si>
-  <si>
-    <t>Marketing Fee Amsterdam (Pay Hotel Expedia)</t>
-  </si>
-  <si>
-    <t>Expedia Marketing Fee Penalty</t>
+    <t>Expedia Marketing Fee</t>
+  </si>
+  <si>
+    <t>Expedia Marketing Fee (Penalty)</t>
+  </si>
+  <si>
+    <t>HT0254</t>
   </si>
 </sst>
 </file>
@@ -417,16 +417,16 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
     <col min="2" max="2" width="49" style="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -465,10 +465,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>505992</v>
@@ -482,10 +482,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>461953</v>
@@ -514,10 +514,10 @@
       <selection sqref="A1:G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.7109375" style="1" customWidth="1"/>
-    <col min="3" max="5" width="11.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.75" style="1" customWidth="1"/>
+    <col min="3" max="5" width="11.25" style="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="1"/>
   </cols>
   <sheetData>

</xml_diff>